<commit_message>
fix accessions with a dash for a range of values
2021.004P.A.v1.Anulavirus_1ns.zip
2021.005P.A.v1.Bromovirus_1ns.zip
2021.010P.A.v1.Emaravirus_1ns.zip
2021.011P.A.v1.Emaravirus_1ns.zip
2021.012P.A.v1.Emaravirus_1ns.zip
</commit_message>
<xml_diff>
--- a/corrections.xlsx
+++ b/corrections.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/curtish/Documents/ICTV/MSL36_load/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/curtish/Documents/ICTV/MSL_merge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BEF96C-7C56-844C-A412-014295A58E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EB3C49-285D-9A41-AAF7-7E714B0964E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="-8860" windowWidth="28040" windowHeight="8680" xr2:uid="{E8C815AD-C1EC-5948-BD5E-7D72C3CFDDC2}"/>
+    <workbookView xWindow="-4800" yWindow="-21100" windowWidth="28040" windowHeight="8680" xr2:uid="{E8C815AD-C1EC-5948-BD5E-7D72C3CFDDC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$7</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="44">
   <si>
     <t>zip</t>
   </si>
@@ -149,6 +149,27 @@
   </si>
   <si>
     <t>CV; Host=Protozoa / environmental; changed to "protozoa; environmental", and updated TP_Template_Excel_module_2022_v2.xlsx</t>
+  </si>
+  <si>
+    <t>2021.004P.A.v1.Anulavirus_1ns.zip</t>
+  </si>
+  <si>
+    <t>ACCESSION range</t>
+  </si>
+  <si>
+    <t>2021.005P.A.v1.Bromovirus_1ns.zip</t>
+  </si>
+  <si>
+    <t>fix3</t>
+  </si>
+  <si>
+    <t>2021.010P.A.v1.Emaravirus_1ns.zip</t>
+  </si>
+  <si>
+    <t>2021.011P.A.v1.Emaravirus_1ns.zip</t>
+  </si>
+  <si>
+    <t>2021.012P.A.v1.Emaravirus_1ns.zip</t>
   </si>
 </sst>
 </file>
@@ -515,11 +536,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AA8345-F56B-3C43-975A-7D2A060B3BB1}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -579,7 +600,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A19" si="0">CONCATENATE("All ",MID(B3,9,1)," proposals")</f>
+        <f t="shared" ref="A3:A24" si="0">CONCATENATE("All ",MID(B3,9,1)," proposals")</f>
         <v>All B proposals</v>
       </c>
       <c r="B3" t="s">
@@ -983,6 +1004,126 @@
       </c>
       <c r="G19" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v>All P proposals</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v>All P proposals</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="str">
+        <f t="shared" si="0"/>
+        <v>All P proposals</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="str">
+        <f t="shared" si="0"/>
+        <v>All P proposals</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="str">
+        <f t="shared" si="0"/>
+        <v>All P proposals</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrections; in process of step 4.a
</commit_message>
<xml_diff>
--- a/corrections.xlsx
+++ b/corrections.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/curtish/Documents/ICTV/MSL_merge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EB3C49-285D-9A41-AAF7-7E714B0964E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AB9367-2AFD-7B49-8FE4-1F588F088F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4800" yWindow="-21100" windowWidth="28040" windowHeight="8680" xr2:uid="{E8C815AD-C1EC-5948-BD5E-7D72C3CFDDC2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" xr2:uid="{E8C815AD-C1EC-5948-BD5E-7D72C3CFDDC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="77">
   <si>
     <t>zip</t>
   </si>
@@ -170,13 +170,190 @@
   </si>
   <si>
     <t>2021.012P.A.v1.Emaravirus_1ns.zip</t>
+  </si>
+  <si>
+    <t>2021.036M.A.v1.Rhabdoviridae_sprename</t>
+  </si>
+  <si>
+    <r>
+      <t>srcSpecies: Culex ohls</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>rha</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rhavirus =&gt; Culex ohlsrhavirus</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>srcSpecies: Bas Congo tibrovirus =&gt; Bas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Congo tibrovirus</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>srcKingdom &amp; kingdom: Orthorna</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>riv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ae =&gt; Orthorna</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>vir</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ae</t>
+    </r>
+  </si>
+  <si>
+    <t>2021.001B.A.v1.abolish_Caudovirales.zip</t>
+  </si>
+  <si>
+    <t>genus:Incheonvrus</t>
+  </si>
+  <si>
+    <t>NO - requires a proposal</t>
+  </si>
+  <si>
+    <t>2021.010B.A.v1.Binomial_names.zip</t>
+  </si>
+  <si>
+    <t>genus:Tunggulviirus; genus:Incheonvrus;</t>
+  </si>
+  <si>
+    <t>2021.039M.A.v1.Xinmoviridae_10ngen_8nsp</t>
+  </si>
+  <si>
+    <t>new genus: Doupovirus (missing)</t>
+  </si>
+  <si>
+    <t>2021.001B.A.v1.abolish_Caudovirales.xlsx</t>
+  </si>
+  <si>
+    <t>fix accidental rename of Stanholtvirus to Squirtyvirus</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>2021.015B.A.v1.Casjensviridae.xlsx</t>
+  </si>
+  <si>
+    <t>delete row for "new species" Chvirus BSPM4 - already created by a rename in 2021.010B</t>
+  </si>
+  <si>
+    <t>2021.076B.A.v1.Schitoviridae_new_genera.xlsx</t>
+  </si>
+  <si>
+    <t>delete rows for new genus/species Glaucusvirus</t>
+  </si>
+  <si>
+    <t>2021.082B.A.v1.Tevens_new_families.xlsx</t>
+  </si>
+  <si>
+    <t>remove genus move of Haloferacalesvirus</t>
+  </si>
+  <si>
+    <t>2021.010B.A.v1.Binomial_names.xlsx</t>
+  </si>
+  <si>
+    <t>remove species rename Haloferax virus HF1 -&gt; Haloferacalesvirus HF1; already done in 2021.001A</t>
+  </si>
+  <si>
+    <t>remove genus move of Myohalovirus; correctly done n 2021.001A</t>
+  </si>
+  <si>
+    <t>remove duplicate species rename Natrialba virus PhiCh1 -&gt; Myohalovirus phiCh1; already done in 2021.001A</t>
+  </si>
+  <si>
+    <t>remove duplicate species rename Halobacterium virus phiH-&gt; Myohalovirus phiH; already done in 2021.001A</t>
+  </si>
+  <si>
+    <t>2021.061B.A.v1.Pbunavirus_new_species</t>
+  </si>
+  <si>
+    <t>remove  new species that duplicates a rename: Pbunavrus BrSP1</t>
+  </si>
+  <si>
+    <t>udpate host, genome on renamed species: Pbunavrus BrSP1</t>
+  </si>
+  <si>
+    <t>remove move_genus Phapecoctavirus</t>
+  </si>
+  <si>
+    <t>remove move_genus psimunavirus</t>
+  </si>
+  <si>
+    <t>remove duplicate genus move for rerduovirus</t>
+  </si>
+  <si>
+    <t>2021.001B.A.v1.abolish_Caudovirales</t>
+  </si>
+  <si>
+    <t>remove duplicate move species Yonseivirus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -198,13 +375,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -219,9 +413,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,22 +732,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AA8345-F56B-3C43-975A-7D2A060B3BB1}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25:XFD25"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -573,8 +769,11 @@
       <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>CONCATENATE("All ",MID(B2,9,1)," proposals")</f>
         <v>All B proposals</v>
@@ -598,9 +797,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A24" si="0">CONCATENATE("All ",MID(B3,9,1)," proposals")</f>
+        <f t="shared" ref="A3:A31" si="0">CONCATENATE("All ",MID(B3,9,1)," proposals")</f>
         <v>All B proposals</v>
       </c>
       <c r="B3" t="s">
@@ -622,7 +821,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>All B proposals</v>
@@ -646,7 +845,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>All D proposals</v>
@@ -670,7 +869,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>All D proposals</v>
@@ -694,7 +893,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>All D proposals</v>
@@ -718,7 +917,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>All D proposals</v>
@@ -742,7 +941,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>All F proposals</v>
@@ -766,7 +965,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>All M proposals</v>
@@ -790,7 +989,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>All M proposals</v>
@@ -814,7 +1013,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>All M proposals</v>
@@ -838,7 +1037,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>All P proposals</v>
@@ -862,7 +1061,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>All P proposals</v>
@@ -886,7 +1085,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>All P proposals</v>
@@ -910,7 +1109,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>All P proposals</v>
@@ -934,7 +1133,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>All P proposals</v>
@@ -958,7 +1157,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>All P proposals</v>
@@ -982,7 +1181,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>All S proposals</v>
@@ -1006,7 +1205,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>All P proposals</v>
@@ -1030,7 +1229,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>All P proposals</v>
@@ -1054,7 +1253,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>All P proposals</v>
@@ -1078,7 +1277,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>All P proposals</v>
@@ -1102,7 +1301,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>All P proposals</v>
@@ -1124,6 +1323,305 @@
       </c>
       <c r="G24" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="str">
+        <f t="shared" si="0"/>
+        <v>All M proposals</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="str">
+        <f t="shared" si="0"/>
+        <v>All M proposals</v>
+      </c>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="str">
+        <f t="shared" si="0"/>
+        <v>All M proposals</v>
+      </c>
+      <c r="B27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="str">
+        <f t="shared" si="0"/>
+        <v>All B proposals</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="str">
+        <f t="shared" si="0"/>
+        <v>All B proposals</v>
+      </c>
+      <c r="B29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" t="s">
+        <v>35</v>
+      </c>
+      <c r="G29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="str">
+        <f t="shared" si="0"/>
+        <v>All M proposals</v>
+      </c>
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="str">
+        <f t="shared" si="0"/>
+        <v>All B proposals</v>
+      </c>
+      <c r="B31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="H35" s="3"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37" s="3"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39" s="3"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41" s="3"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" t="s">
+        <v>76</v>
+      </c>
+      <c r="D45" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct SQL out filename variable
</commit_message>
<xml_diff>
--- a/corrections.xlsx
+++ b/corrections.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/curtish/Documents/ICTV/validate_proposals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B912711E-3832-0A43-B3AF-A19EC5733657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A131DC67-5641-B646-BDB0-BE593D87EE45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16520" xr2:uid="{E8C815AD-C1EC-5948-BD5E-7D72C3CFDDC2}"/>
   </bookViews>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
   <si>
     <t>fix</t>
   </si>
@@ -306,13 +306,34 @@
   </si>
   <si>
     <t>moves "Melon Tenuivirus" to "Mechlorovirus" and renames it "Mechlorovirus cucumeris", but 2021.002M.A.v2.Phenuiviridae_sprenamed.xlsx:116 renamed it "Tenuivirus cucumeris", too</t>
+  </si>
+  <si>
+    <t>2022.016P.A.Cilevirus_3ns[ ].docx</t>
+  </si>
+  <si>
+    <t>DOCX_FILENAME_SPACES</t>
+  </si>
+  <si>
+    <t>replaced spaces with underscore</t>
+  </si>
+  <si>
+    <t>delete space before period-docx</t>
+  </si>
+  <si>
+    <t>2022.001M.Alpha[_]and[_]betanucleorhabdoviruses_6nsp.*</t>
+  </si>
+  <si>
+    <t>2022.003B.Abolish[_]Haartmanvirus.*</t>
+  </si>
+  <si>
+    <t>2022.016P.A.v1.Cilevirus_3ns[ ].docx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -361,6 +382,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -382,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -393,7 +420,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -403,10 +429,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,11 +745,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AA8345-F56B-3C43-975A-7D2A060B3BB1}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -733,7 +757,7 @@
     <col min="1" max="1" width="82" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.83203125" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="45.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -747,7 +771,7 @@
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -768,7 +792,7 @@
       <c r="C2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -782,7 +806,7 @@
       <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -799,7 +823,7 @@
       <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -816,7 +840,7 @@
       <c r="C5">
         <v>5</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -830,7 +854,7 @@
       <c r="C6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -844,7 +868,7 @@
       <c r="C7">
         <v>14</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -858,7 +882,7 @@
       <c r="C8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -869,13 +893,13 @@
       <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" t="s">
         <v>47</v>
       </c>
       <c r="C9">
         <v>9</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -892,7 +916,7 @@
       <c r="C10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -906,10 +930,10 @@
       <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="9">
         <v>103126</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>49</v>
       </c>
       <c r="E11" t="s">
@@ -926,7 +950,7 @@
       <c r="C12" s="5">
         <v>14</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>36</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -937,13 +961,13 @@
       <c r="A13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13">
         <v>21</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="7" t="s">
         <v>43</v>
       </c>
       <c r="E13" t="s">
@@ -957,7 +981,7 @@
       <c r="C14" s="3">
         <v>4</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -968,13 +992,13 @@
       <c r="A15" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="7" t="s">
         <v>46</v>
       </c>
       <c r="E15" t="s">
@@ -982,14 +1006,73 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>51</v>
       </c>
       <c r="C16">
         <v>16</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>